<commit_message>
Atualização do Cronograma e alerta no login
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>João Otávio</t>
   </si>
@@ -53,6 +53,33 @@
   </si>
   <si>
     <t>Projeto CESEC</t>
+  </si>
+  <si>
+    <t>Relatorio alunos X Disciplina e geral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relatorio alunos X Materia / Nível </t>
+  </si>
+  <si>
+    <t>Relatorio alunos concluinte</t>
+  </si>
+  <si>
+    <t>Relatorio Discplina por tempo</t>
+  </si>
+  <si>
+    <t>Relatorio Frequencia tempo (Disciplina e Geral)</t>
+  </si>
+  <si>
+    <t>Relatorio Media por disciplina e nível</t>
+  </si>
+  <si>
+    <t>CRUD Nota</t>
+  </si>
+  <si>
+    <t>CRUD Frequencia</t>
+  </si>
+  <si>
+    <t>Testes finais e entrega</t>
   </si>
 </sst>
 </file>
@@ -77,23 +104,21 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="11"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,12 +128,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,8 +161,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -348,52 +379,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,75 +762,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L20"/>
+  <dimension ref="B3:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="13">
         <v>43404</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <v>43411</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <v>43418</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="13">
         <v>43425</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="13">
         <v>43432</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="13">
         <v>43439</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="14">
         <v>43446</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2"/>
@@ -775,161 +839,199 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="10"/>
-      <c r="K7" s="8" t="s">
+      <c r="I7" s="9"/>
+      <c r="K7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="10"/>
-      <c r="K8" s="8" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="9"/>
+      <c r="K8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="10"/>
-      <c r="K9" s="9" t="s">
+      <c r="I9" s="9"/>
+      <c r="K9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="10"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="10"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="10"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>11</v>
+      <c r="B13" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="10"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
+      <c r="B14" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="10"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
+      <c r="B15" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="10"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
+      <c r="B16" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
+      <c r="B17" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="10"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
+      <c r="B18" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="10"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
+      <c r="B19" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="5"/>
     </row>
   </sheetData>
   <sortState ref="K9:K11">

</xml_diff>

<commit_message>
Arrumando o layout do cadastro de aluno, atualizando cronograma e iniciando o cadstro da matricula
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>João Otávio</t>
   </si>
@@ -80,13 +80,25 @@
   </si>
   <si>
     <t>Testes finais e entrega</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Atrasado</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +125,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -409,18 +427,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -430,6 +444,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -448,16 +463,52 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +816,7 @@
   <dimension ref="B3:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,260 +829,278 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="9">
         <v>43404</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="9">
         <v>43411</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="9">
         <v>43418</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="9">
         <v>43425</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="9">
         <v>43432</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="9">
         <v>43439</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="10">
         <v>43446</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L6" s="1"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="9"/>
-      <c r="K7" s="7" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
+      <c r="K7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="9"/>
-      <c r="K8" s="7" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="22"/>
+      <c r="K8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="26"/>
+      <c r="L8" s="12"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="9"/>
-      <c r="K9" s="8" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+      <c r="K9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="9"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="22"/>
+      <c r="K10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="9"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="K11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="9"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="9"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="9"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="9"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="9"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="9"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="9"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="9"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="29"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="29"/>
     </row>
     <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="31"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="5"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="33"/>
     </row>
   </sheetData>
   <sortState ref="K9:K11">

</xml_diff>

<commit_message>
Mudança da ideia de secretária para atributo de professor
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>João Otávio</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Jonas</t>
+  </si>
+  <si>
+    <t>CRUD Secretárias</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -508,11 +511,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -623,6 +637,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -929,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P22"/>
+  <dimension ref="B3:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,23 +1211,23 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="48"/>
       <c r="K15" s="33"/>
       <c r="L15" s="16"/>
       <c r="M15" s="40"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1226,7 +1243,7 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1242,7 +1259,7 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1258,7 +1275,7 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1274,23 +1291,23 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="22"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="16"/>
       <c r="M20" s="40"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -1304,21 +1321,37 @@
       <c r="L21" s="22"/>
       <c r="M21" s="40"/>
     </row>
-    <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="40"/>
+    </row>
+    <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="41"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="41"/>
     </row>
   </sheetData>
   <sortState ref="O9:O11">

</xml_diff>